<commit_message>
Fichier excel mise à jour à utiliser pour la suite du projet
</commit_message>
<xml_diff>
--- a/Donnees/fichier_mis_a_jour.xlsx
+++ b/Donnees/fichier_mis_a_jour.xlsx
@@ -45916,7 +45916,9 @@
       <c r="AN333" t="inlineStr"/>
     </row>
     <row r="334">
-      <c r="A334" t="inlineStr"/>
+      <c r="A334" t="n">
+        <v>407</v>
+      </c>
       <c r="B334" t="inlineStr">
         <is>
           <t>PeepSpace</t>
@@ -45978,7 +45980,9 @@
       </c>
     </row>
     <row r="335">
-      <c r="A335" t="inlineStr"/>
+      <c r="A335" t="n">
+        <v>408</v>
+      </c>
       <c r="B335" t="inlineStr">
         <is>
           <t>Kurt-forever</t>
@@ -46041,7 +46045,9 @@
       </c>
     </row>
     <row r="336">
-      <c r="A336" t="inlineStr"/>
+      <c r="A336" t="n">
+        <v>409</v>
+      </c>
       <c r="B336" t="inlineStr">
         <is>
           <t>Palais des paris</t>
@@ -46107,7 +46113,9 @@
       </c>
     </row>
     <row r="337">
-      <c r="A337" t="inlineStr"/>
+      <c r="A337" t="n">
+        <v>410</v>
+      </c>
       <c r="B337" t="inlineStr">
         <is>
           <t>GLASSBOX-NORD</t>

</xml_diff>